<commit_message>
updated Vol column name to Volatility
</commit_message>
<xml_diff>
--- a/data/plan_inputs/output.xlsx
+++ b/data/plan_inputs/output.xlsx
@@ -5,19 +5,30 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\NVG9HXP\Documents\Projects\UPS_MV\data\outputs\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\NVG9HXP\Documents\Projects\UPS_MV\data\plan_inputs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2D8EC3BD-093D-4BA1-B67F-D0B405EBDF49}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{51BBA602-DF7F-4F07-81B0-8F65C870A277}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="ret_vol" sheetId="1" r:id="rId1"/>
     <sheet name="corr" sheetId="2" r:id="rId2"/>
     <sheet name="weights" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="124519"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
@@ -27,9 +38,6 @@
     <t>Return</t>
   </si>
   <si>
-    <t>Vol</t>
-  </si>
-  <si>
     <t>Liability</t>
   </si>
   <si>
@@ -73,6 +81,9 @@
   </si>
   <si>
     <t>FS AdjWeights</t>
+  </si>
+  <si>
+    <t>Volatility</t>
   </si>
 </sst>
 </file>
@@ -501,7 +512,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:ALM12"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C1" sqref="C1"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -513,12 +526,12 @@
         <v>0</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>1</v>
+        <v>16</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B2" s="1">
         <v>9.2548370471084107E-2</v>
@@ -529,7 +542,7 @@
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B3" s="1">
         <v>9.0032396370271828E-2</v>
@@ -540,7 +553,7 @@
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B4" s="1">
         <v>7.5283545176406452E-2</v>
@@ -551,7 +564,7 @@
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B5" s="1">
         <v>5.3655865973994521E-2</v>
@@ -562,7 +575,7 @@
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B6" s="1">
         <v>0.1049948122760576</v>
@@ -573,7 +586,7 @@
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B7" s="1">
         <v>1.5921210926720161E-2</v>
@@ -584,7 +597,7 @@
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B8" s="1">
         <v>0.14531713352338249</v>
@@ -595,7 +608,7 @@
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B9" s="1">
         <v>5.7278383542747058E-2</v>
@@ -606,7 +619,7 @@
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B10" s="1">
         <v>0.1141442099228849</v>
@@ -617,7 +630,7 @@
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B11" s="1">
         <v>5.7081799836757874E-3</v>
@@ -628,7 +641,7 @@
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B12" s="1">
         <v>2.250840125906417E-2</v>
@@ -644,6 +657,7 @@
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -660,42 +674,42 @@
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="D1" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="E1" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="F1" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="F1" s="2" t="s">
+      <c r="G1" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="G1" s="2" t="s">
+      <c r="H1" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="H1" s="2" t="s">
+      <c r="I1" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="I1" s="2" t="s">
+      <c r="J1" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="J1" s="2" t="s">
+      <c r="K1" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="K1" s="2" t="s">
+      <c r="L1" s="2" t="s">
         <v>11</v>
-      </c>
-      <c r="L1" s="2" t="s">
-        <v>12</v>
       </c>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B2" s="1">
         <v>1</v>
@@ -733,7 +747,7 @@
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B3" s="1">
         <v>0.78500417574812575</v>
@@ -771,7 +785,7 @@
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B4" s="1">
         <v>0.90025671245448913</v>
@@ -809,7 +823,7 @@
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B5" s="1">
         <v>0.77581921911589324</v>
@@ -847,7 +861,7 @@
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B6" s="1">
         <v>4.5897125584404487E-2</v>
@@ -885,7 +899,7 @@
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B7" s="1">
         <v>0.3290946389236713</v>
@@ -923,7 +937,7 @@
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B8" s="1">
         <v>-2.600878819886502E-2</v>
@@ -961,7 +975,7 @@
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B9" s="1">
         <v>0.2129921075867674</v>
@@ -999,7 +1013,7 @@
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B10" s="1">
         <v>0.14862038047415391</v>
@@ -1037,7 +1051,7 @@
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B11" s="1">
         <v>-2.024689421365582E-2</v>
@@ -1075,7 +1089,7 @@
     </row>
     <row r="12" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B12" s="1">
         <v>-0.1799984172038111</v>
@@ -1123,7 +1137,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6F492546-F42B-45A4-BB39-613EE8942B10}">
   <dimension ref="A1:ALM12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -1132,21 +1146,21 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="B1" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="C1" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="D1" s="2" t="s">
         <v>15</v>
-      </c>
-      <c r="D1" s="2" t="s">
-        <v>16</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B2" s="1">
         <v>-1</v>
@@ -1160,7 +1174,7 @@
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B3" s="1">
         <v>0.14000000000000001</v>
@@ -1174,7 +1188,7 @@
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B4" s="1">
         <v>0.14000000000000001</v>
@@ -1188,7 +1202,7 @@
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B5" s="1">
         <v>0</v>
@@ -1202,7 +1216,7 @@
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B6" s="1">
         <v>0.43</v>
@@ -1216,7 +1230,7 @@
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B7" s="1">
         <v>0.09</v>
@@ -1230,7 +1244,7 @@
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B8" s="1">
         <v>0.08</v>
@@ -1244,7 +1258,7 @@
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B9" s="1">
         <v>0.05</v>
@@ -1258,7 +1272,7 @@
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B10" s="1">
         <v>0.05</v>
@@ -1272,7 +1286,7 @@
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B11" s="1">
         <v>0.02</v>
@@ -1286,7 +1300,7 @@
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B12" s="1">
         <v>0</v>

</xml_diff>